<commit_message>
Completing mod 1 and part of final exam
</commit_message>
<xml_diff>
--- a/Module 1 - Quiz/Module 1_Quiz Data_Income.xlsx
+++ b/Module 1 - Quiz/Module 1_Quiz Data_Income.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17668"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CertTFS\Online-Content\Courses\ENG\DAT222x - Essential Statistics for Data Analysis using Excel\Assessments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anguyen\Documents\GitHub\stats-edx\Module 1 - Quiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1C65B9-DF1C-45CF-80C5-9222EDAEBD40}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11978"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -38,7 +44,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -109,37 +115,7 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <numFmt numFmtId="32" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
       <fill>
@@ -185,12 +161,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:C11" totalsRowShown="0">
-  <autoFilter ref="A3:C11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:C11" totalsRowShown="0">
+  <autoFilter ref="A3:C11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A4:C11">
+    <sortCondition ref="B3:B11"/>
+  </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Year"/>
-    <tableColumn id="2" name="Median in 2015 dollars" dataDxfId="4" dataCellStyle="Currency"/>
-    <tableColumn id="3" name="Mean in 2015 dollars" dataDxfId="3" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Year"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Median in 2015 dollars" dataDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Mean in 2015 dollars" dataDxfId="0" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -492,20 +471,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B4" sqref="B4:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.19921875" customWidth="1"/>
-    <col min="3" max="3" width="8.73046875" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -516,62 +495,62 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4" s="2">
+        <v>52666</v>
+      </c>
+      <c r="C4" s="3">
+        <v>75825</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2011</v>
+      </c>
+      <c r="B5" s="2">
+        <v>52751</v>
+      </c>
+      <c r="C5" s="3">
+        <v>75325</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2010</v>
+      </c>
+      <c r="B6" s="2">
+        <v>53568</v>
+      </c>
+      <c r="C6" s="3">
+        <v>75093</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>2014</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B7" s="2">
         <v>53719</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C7" s="3">
         <v>77286</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>2013</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B8" s="2">
         <v>54525</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C8" s="3">
         <v>76513</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>2012</v>
-      </c>
-      <c r="B6" s="2">
-        <v>52666</v>
-      </c>
-      <c r="C6" s="3">
-        <v>75825</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>2011</v>
-      </c>
-      <c r="B7" s="2">
-        <v>52751</v>
-      </c>
-      <c r="C7" s="3">
-        <v>75325</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>2010</v>
-      </c>
-      <c r="B8" s="2">
-        <v>53568</v>
-      </c>
-      <c r="C8" s="3">
-        <v>75093</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2009</v>
       </c>
@@ -582,7 +561,7 @@
         <v>73577</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -593,7 +572,7 @@
         <v>73431</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2007</v>
       </c>

</xml_diff>